<commit_message>
tambah API address dan edit middleware member
</commit_message>
<xml_diff>
--- a/Target dan Jadwal.xlsx
+++ b/Target dan Jadwal.xlsx
@@ -737,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E1:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:Q36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1477,6 +1477,6 @@
     <mergeCell ref="K4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967294" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>